<commit_message>
:recycle: refactor: Melhorias relacionadas a filtro e edicao de certificado
</commit_message>
<xml_diff>
--- a/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-FRANCISCO JEAN DOS SANTOS ESTEVAM.xlsx
+++ b/media/ficha/Termo de Responsabilidade Equipamentos de Medição_Atualizado-FRANCISCO JEAN DOS SANTOS ESTEVAM.xlsx
@@ -802,6 +802,31 @@
   </oneCellAnchor>
   <oneCellAnchor>
     <from>
+      <col>9</col>
+      <colOff>0</colOff>
+      <row>19</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1619250" cy="762000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
       <col>3</col>
       <colOff>0</colOff>
       <row>11</row>
@@ -810,11 +835,11 @@
     <ext cx="952500" cy="476250"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1357,29 +1382,75 @@
       <c r="J18" s="17" t="n"/>
       <c r="K18" s="86" t="n"/>
     </row>
-    <row r="19" ht="12.75" customHeight="1" s="6">
-      <c r="A19" s="7" t="n"/>
-      <c r="B19" s="7" t="n"/>
-      <c r="C19" s="7" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="7" t="n"/>
-      <c r="G19" s="7" t="n"/>
-      <c r="H19" s="7" t="n"/>
-      <c r="I19" s="7" t="n"/>
-      <c r="J19" s="7" t="n"/>
-      <c r="K19" s="7" t="n"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1" s="6">
-      <c r="A20" s="7" t="n"/>
-      <c r="B20" s="7" t="n"/>
-      <c r="C20" s="7" t="n"/>
-      <c r="E20" s="7" t="n"/>
-      <c r="F20" s="7" t="n"/>
-      <c r="G20" s="7" t="n"/>
-      <c r="H20" s="7" t="n"/>
-      <c r="I20" s="7" t="n"/>
-      <c r="J20" s="7" t="n"/>
-      <c r="K20" s="7" t="n"/>
+    <row r="19" ht="57.75" customHeight="1" s="6">
+      <c r="A19" s="17" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+      <c r="B19" s="17" t="inlineStr">
+        <is>
+          <t>Balança DIGI-TRON ULD20000</t>
+        </is>
+      </c>
+      <c r="C19" s="85" t="n"/>
+      <c r="D19" s="86" t="n"/>
+      <c r="E19" s="17" t="inlineStr">
+        <is>
+          <t>BAL-CQ-002</t>
+        </is>
+      </c>
+      <c r="F19" s="86" t="n"/>
+      <c r="G19" s="18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0 - 20000</t>
+        </is>
+      </c>
+      <c r="H19" s="61" t="inlineStr">
+        <is>
+          <t>substituição - calibração</t>
+        </is>
+      </c>
+      <c r="I19" s="17" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+      <c r="J19" s="17" t="n"/>
+      <c r="K19" s="86" t="n"/>
+    </row>
+    <row r="20" ht="57.75" customHeight="1" s="6">
+      <c r="A20" s="17" t="inlineStr">
+        <is>
+          <t>08/07/2025</t>
+        </is>
+      </c>
+      <c r="B20" s="17" t="inlineStr">
+        <is>
+          <t>Balança WT1000</t>
+        </is>
+      </c>
+      <c r="C20" s="85" t="n"/>
+      <c r="D20" s="86" t="n"/>
+      <c r="E20" s="17" t="inlineStr">
+        <is>
+          <t>BAL-CQ-001</t>
+        </is>
+      </c>
+      <c r="F20" s="86" t="n"/>
+      <c r="G20" s="18" t="inlineStr">
+        <is>
+          <t>0 - 50000</t>
+        </is>
+      </c>
+      <c r="H20" s="61" t="inlineStr">
+        <is>
+          <t>Entrega</t>
+        </is>
+      </c>
+      <c r="I20" s="17" t="n"/>
+      <c r="J20" s="17" t="n"/>
+      <c r="K20" s="86" t="n"/>
     </row>
     <row r="21" ht="12.75" customHeight="1" s="6">
       <c r="A21" s="7" t="n"/>
@@ -1396,17 +1467,23 @@
     </row>
     <row r="22" ht="15.75" customHeight="1" s="6"/>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="30">
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="J19:K19"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="K1:K4"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="C3:G4"/>
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="G12:I12"/>

</xml_diff>